<commit_message>
Add similarity vs local area density graph between images
</commit_message>
<xml_diff>
--- a/MySEProject/Dataset Reports/Dataset-GurunagSai/Experiment Report.xlsx
+++ b/MySEProject/Dataset Reports/Dataset-GurunagSai/Experiment Report.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gurunag Sai\source\repos\neocortexapi-classification\MySEProject\Dataset Reports\Dataset-GurunagSai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52CF7F2E-AF4B-409B-9A65-413B6A06D8DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600AB0B3-82EC-4930-B127-B0301B782767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="144">
   <si>
     <t>Experiment Number</t>
   </si>
@@ -488,15 +491,26 @@
     <t>Better output micro(92-75) and macro(68-45)</t>
   </si>
   <si>
-    <t>Similarities between two images</t>
-  </si>
-  <si>
     <t>rectangle0_rectangle_2
-input sim: 61.11</t>
-  </si>
-  <si>
-    <t>rectangle0__triangle1
-input sim: 38.63</t>
+input similarity</t>
+  </si>
+  <si>
+    <t>rectangle0_rectangle_2
+output similarity</t>
+  </si>
+  <si>
+    <t>Output Similarities between two images</t>
+  </si>
+  <si>
+    <t>Input similarities between two images</t>
+  </si>
+  <si>
+    <t>rectangle0__triangle0
+Input Similarity</t>
+  </si>
+  <si>
+    <t>rectangle0__triangle0
+output similarity</t>
   </si>
 </sst>
 </file>
@@ -622,7 +636,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -676,6 +690,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,6 +708,3367 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Output Similarity Between Rectangle0 &amp; Rectangle2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14128909735050552"/>
+          <c:y val="2.7213819191670999E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12206686319973774"/>
+          <c:y val="0.13936499183823514"/>
+          <c:w val="0.80218687259449561"/>
+          <c:h val="0.61675823652546913"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Potential Radius=5</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$4:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$49:$J$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>18.12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39.450000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>78.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95.24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>98.69</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-D342-4C52-8EEA-BED64FAE3DCD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Potential Radius=10</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$4:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$36:$J$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>29.41</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>76.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>84.73</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-D342-4C52-8EEA-BED64FAE3DCD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Potential Radius=15</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$4:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$30:$J$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>73.239999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75.89</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>88.36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>87.14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>96.49</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-D342-4C52-8EEA-BED64FAE3DCD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Potential Radius=20</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$4:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$23:$J$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>71.08</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80.44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>85.13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90.14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>93.91</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D342-4C52-8EEA-BED64FAE3DCD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Potential Radius=30</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$4:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$4:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>63.55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>84.66</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>99.89</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D342-4C52-8EEA-BED64FAE3DCD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>input similarity</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$4:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$4:$L$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>61.11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>61.11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>61.11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>61.11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>61.11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D342-4C52-8EEA-BED64FAE3DCD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1624190000"/>
+        <c:axId val="1624203728"/>
+        <c:extLst/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1624190000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>Local Area Density</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1624203728"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1624203728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>Similarity in %</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1624190000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Output Similarity Between Rectangle0 &amp; Triangle0</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14128909735050552"/>
+          <c:y val="2.7213819191670999E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12206686319973774"/>
+          <c:y val="0.1484362649021255"/>
+          <c:w val="0.80218687259449561"/>
+          <c:h val="0.61675823652546913"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Potential Radius=5</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$4:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$49:$K$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>20.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>79.14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95.46</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>99.09</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-C274-4A7F-A722-06D126AFC136}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Potential Radius=10</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$4:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$36:$K$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>22.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27.32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>77.77</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85.72</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97.08</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-C274-4A7F-A722-06D126AFC136}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Potential Radius=15</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$4:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$30:$K$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>43.29</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52.23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>77.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80.36</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>94.58</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-C274-4A7F-A722-06D126AFC136}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Potential Radius=20</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$4:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$23:$K$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>46.27</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42.13</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64.16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>75.290000000000006</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90.72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C274-4A7F-A722-06D126AFC136}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Potential Radius=30</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$4:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$4:$K$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>21.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>48.46</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80.48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>99.78</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C274-4A7F-A722-06D126AFC136}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>input similarity</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$4:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$4:$M$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>38.630000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38.630000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>38.630000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38.630000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38.630000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C274-4A7F-A722-06D126AFC136}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1624190000"/>
+        <c:axId val="1624203728"/>
+        <c:extLst/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1624190000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Local Area Density</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1624203728"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1624203728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Similarity in %</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1624190000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>5562600</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>699861</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>56697</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39812E4F-B154-4C82-9AD6-62B3A6C4F75B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>433161</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>37647</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E3F16A2-CABA-4A68-B2E3-5FF7CB78C575}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Tabelle1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="B2">
+            <v>0.1</v>
+          </cell>
+          <cell r="D2">
+            <v>37.464788732394297</v>
+          </cell>
+          <cell r="F2">
+            <v>27.358490566037698</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="B3">
+            <v>0.2</v>
+          </cell>
+          <cell r="D3">
+            <v>37.464788732394297</v>
+          </cell>
+          <cell r="F3">
+            <v>47.783251231526997</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4">
+            <v>0.3</v>
+          </cell>
+          <cell r="D4">
+            <v>37.464788732394297</v>
+          </cell>
+          <cell r="F4">
+            <v>58.609271523178798</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5">
+            <v>0.4</v>
+          </cell>
+          <cell r="D5">
+            <v>37.464788732394297</v>
+          </cell>
+          <cell r="F5">
+            <v>69.343065693430603</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6">
+            <v>0.5</v>
+          </cell>
+          <cell r="D6">
+            <v>37.464788732394297</v>
+          </cell>
+          <cell r="F6">
+            <v>78.285714285714207</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7">
+            <v>0.6</v>
+          </cell>
+          <cell r="D7">
+            <v>37.464788732394297</v>
+          </cell>
+          <cell r="F7">
+            <v>84.815950920245399</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8">
+            <v>0.7</v>
+          </cell>
+          <cell r="D8">
+            <v>37.464788732394297</v>
+          </cell>
+          <cell r="F8">
+            <v>91.912708600770202</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9">
+            <v>0.8</v>
+          </cell>
+          <cell r="D9">
+            <v>37.464788732394297</v>
+          </cell>
+          <cell r="F9">
+            <v>95.744680851063805</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10">
+            <v>0.9</v>
+          </cell>
+          <cell r="D10">
+            <v>37.464788732394297</v>
+          </cell>
+          <cell r="F10">
+            <v>99.1718426501035</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11">
+            <v>1</v>
+          </cell>
+          <cell r="D11">
+            <v>37.464788732394297</v>
+          </cell>
+          <cell r="F11">
+            <v>100</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="F13">
+            <v>67.741935483870904</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="F14">
+            <v>63.5555555555555</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="F15">
+            <v>75.667655786350096</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="F16">
+            <v>75.963718820861601</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="F17">
+            <v>79.197080291970806</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="F18">
+            <v>80.9672386895475</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="F19">
+            <v>84.7411444141689</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="F20">
+            <v>87.620192307692307</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="F21">
+            <v>92.4160346695557</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="F22">
+            <v>100</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="F24">
+            <v>20.5607476635514</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="F25">
+            <v>44.075829383886202</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="F26">
+            <v>54.807692307692299</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="F27">
+            <v>70.503597122302097</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="F28">
+            <v>75</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="F29">
+            <v>83.144246353322501</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="F30">
+            <v>89.972144846796596</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="F31">
+            <v>92.9095354523227</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="F32">
+            <v>96.637744034707097</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="F33">
+            <v>100</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="F35">
+            <v>45.238095238095198</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="F36">
+            <v>66.992665036674794</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="F37">
+            <v>71.343873517786506</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="F38">
+            <v>82.819383259911802</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="F39">
+            <v>93.280182232346206</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="F40">
+            <v>93.142857142857096</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="F41">
+            <v>96.504237288135599</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="F42">
+            <v>97.971602434076999</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="F43">
+            <v>99.312377210216098</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="F44">
+            <v>100</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="F46">
+            <v>18.627450980392101</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="F47">
+            <v>38.048780487804798</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="F48">
+            <v>54.397394136807797</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="F49">
+            <v>63.414634146341399</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="F50">
+            <v>71.484375</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="F51">
+            <v>80.781758957654702</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="F52">
+            <v>86.610878661087796</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="F53">
+            <v>91.452991452991398</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="F54">
+            <v>97.180043383947904</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="F55">
+            <v>100</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -956,10 +4334,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K73"/>
+  <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="I64" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -976,10 +4354,11 @@
     <col min="10" max="10" width="23.28515625" style="2" customWidth="1"/>
     <col min="11" max="11" width="22.7109375" style="2" customWidth="1"/>
     <col min="12" max="12" width="23" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="2"/>
+    <col min="13" max="13" width="21" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -996,11 +4375,15 @@
         <v>61</v>
       </c>
       <c r="J1" s="18" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="K1" s="19"/>
-    </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L1" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="M1" s="19"/>
+    </row>
+    <row r="2" spans="1:13" s="4" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
       <c r="B2" s="4" t="s">
         <v>4</v>
@@ -1026,15 +4409,21 @@
         <v>139</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="9" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="9" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1063,13 +4452,19 @@
         <v>15</v>
       </c>
       <c r="J4" s="2">
-        <v>4.5</v>
+        <v>24.5</v>
       </c>
       <c r="K4" s="2">
-        <v>11.7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>21.7</v>
+      </c>
+      <c r="L4" s="2">
+        <v>61.11</v>
+      </c>
+      <c r="M4" s="2">
+        <v>38.630000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -1103,8 +4498,14 @@
       <c r="K5" s="2">
         <v>28.3</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L5" s="2">
+        <v>61.11</v>
+      </c>
+      <c r="M5" s="2">
+        <v>38.630000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -1138,8 +4539,14 @@
       <c r="K6" s="2">
         <v>48.46</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L6" s="2">
+        <v>61.11</v>
+      </c>
+      <c r="M6" s="2">
+        <v>38.630000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -1173,8 +4580,14 @@
       <c r="K7" s="20">
         <v>80.48</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L7" s="2">
+        <v>61.11</v>
+      </c>
+      <c r="M7" s="2">
+        <v>38.630000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -1208,8 +4621,14 @@
       <c r="K8" s="2">
         <v>99.78</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L8" s="2">
+        <v>61.11</v>
+      </c>
+      <c r="M8" s="2">
+        <v>38.630000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>22</v>
       </c>
@@ -1238,7 +4657,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>23</v>
       </c>
@@ -1267,7 +4686,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>24</v>
       </c>
@@ -1296,7 +4715,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>25</v>
       </c>
@@ -1325,7 +4744,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>26</v>
       </c>
@@ -1354,7 +4773,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>27</v>
       </c>
@@ -1383,7 +4802,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>28</v>
       </c>
@@ -1412,7 +4831,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>29</v>
       </c>
@@ -1441,7 +4860,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>30</v>
       </c>
@@ -1470,7 +4889,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>31</v>
       </c>
@@ -1499,7 +4918,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>33</v>
       </c>
@@ -1528,7 +4947,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>34</v>
       </c>
@@ -1557,7 +4976,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>35</v>
       </c>
@@ -1586,12 +5005,12 @@
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="9" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" s="9" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>6</v>
       </c>
@@ -1619,8 +5038,20 @@
       <c r="I23" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J23" s="2">
+        <v>71.08</v>
+      </c>
+      <c r="K23" s="2">
+        <v>46.27</v>
+      </c>
+      <c r="L23" s="2">
+        <v>61.11</v>
+      </c>
+      <c r="M23" s="2">
+        <v>38.630000000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>7</v>
       </c>
@@ -1648,8 +5079,20 @@
       <c r="I24" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J24" s="2">
+        <v>80.44</v>
+      </c>
+      <c r="K24" s="2">
+        <v>42.13</v>
+      </c>
+      <c r="L24" s="2">
+        <v>61.11</v>
+      </c>
+      <c r="M24" s="2">
+        <v>38.630000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>8</v>
       </c>
@@ -1677,8 +5120,20 @@
       <c r="I25" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J25" s="2">
+        <v>85.13</v>
+      </c>
+      <c r="K25" s="2">
+        <v>64.16</v>
+      </c>
+      <c r="L25" s="2">
+        <v>61.11</v>
+      </c>
+      <c r="M25" s="2">
+        <v>38.630000000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>9</v>
       </c>
@@ -1712,8 +5167,14 @@
       <c r="K26" s="2">
         <v>75.290000000000006</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L26" s="2">
+        <v>61.11</v>
+      </c>
+      <c r="M26" s="2">
+        <v>38.630000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>10</v>
       </c>
@@ -1741,8 +5202,20 @@
       <c r="I27" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J27" s="2">
+        <v>93.91</v>
+      </c>
+      <c r="K27" s="2">
+        <v>90.72</v>
+      </c>
+      <c r="L27" s="2">
+        <v>61.11</v>
+      </c>
+      <c r="M27" s="2">
+        <v>38.630000000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>32</v>
       </c>
@@ -1771,7 +5244,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="9" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" s="9" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>132</v>
       </c>
@@ -1784,7 +5257,7 @@
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
     </row>
-    <row r="30" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>11</v>
       </c>
@@ -1812,8 +5285,20 @@
       <c r="I30" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J30" s="20">
+        <v>73.239999999999995</v>
+      </c>
+      <c r="K30" s="20">
+        <v>43.29</v>
+      </c>
+      <c r="L30" s="2">
+        <v>61.11</v>
+      </c>
+      <c r="M30" s="2">
+        <v>38.630000000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>12</v>
       </c>
@@ -1841,8 +5326,20 @@
       <c r="I31" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J31" s="20">
+        <v>75.89</v>
+      </c>
+      <c r="K31" s="20">
+        <v>52.23</v>
+      </c>
+      <c r="L31" s="2">
+        <v>61.11</v>
+      </c>
+      <c r="M31" s="2">
+        <v>38.630000000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>13</v>
       </c>
@@ -1870,8 +5367,20 @@
       <c r="I32" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J32" s="20">
+        <v>88.36</v>
+      </c>
+      <c r="K32" s="20">
+        <v>77.599999999999994</v>
+      </c>
+      <c r="L32" s="2">
+        <v>61.11</v>
+      </c>
+      <c r="M32" s="2">
+        <v>38.630000000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>14</v>
       </c>
@@ -1899,8 +5408,20 @@
       <c r="I33" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J33" s="20">
+        <v>87.14</v>
+      </c>
+      <c r="K33" s="20">
+        <v>80.36</v>
+      </c>
+      <c r="L33" s="2">
+        <v>61.11</v>
+      </c>
+      <c r="M33" s="2">
+        <v>38.630000000000003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>15</v>
       </c>
@@ -1928,13 +5449,25 @@
       <c r="I34" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" s="9" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J34" s="20">
+        <v>96.49</v>
+      </c>
+      <c r="K34" s="20">
+        <v>94.58</v>
+      </c>
+      <c r="L34" s="2">
+        <v>61.11</v>
+      </c>
+      <c r="M34" s="2">
+        <v>38.630000000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" s="9" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>16</v>
       </c>
@@ -1962,8 +5495,20 @@
       <c r="I36" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J36" s="20">
+        <v>29.41</v>
+      </c>
+      <c r="K36" s="20">
+        <v>22.1</v>
+      </c>
+      <c r="L36" s="2">
+        <v>61.11</v>
+      </c>
+      <c r="M36" s="2">
+        <v>38.630000000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>17</v>
       </c>
@@ -1991,8 +5536,20 @@
       <c r="I37" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J37" s="2">
+        <v>46.05</v>
+      </c>
+      <c r="K37" s="2">
+        <v>27.32</v>
+      </c>
+      <c r="L37" s="2">
+        <v>61.11</v>
+      </c>
+      <c r="M37" s="2">
+        <v>38.630000000000003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>18</v>
       </c>
@@ -2020,8 +5577,20 @@
       <c r="I38" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J38" s="2">
+        <v>76.900000000000006</v>
+      </c>
+      <c r="K38" s="2">
+        <v>77.77</v>
+      </c>
+      <c r="L38" s="2">
+        <v>61.11</v>
+      </c>
+      <c r="M38" s="2">
+        <v>38.630000000000003</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>19</v>
       </c>
@@ -2049,8 +5618,20 @@
       <c r="I39" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J39" s="2">
+        <v>84.73</v>
+      </c>
+      <c r="K39" s="2">
+        <v>85.72</v>
+      </c>
+      <c r="L39" s="2">
+        <v>61.11</v>
+      </c>
+      <c r="M39" s="2">
+        <v>38.630000000000003</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>20</v>
       </c>
@@ -2078,8 +5659,20 @@
       <c r="I40" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J40" s="2">
+        <v>97.8</v>
+      </c>
+      <c r="K40" s="2">
+        <v>97.08</v>
+      </c>
+      <c r="L40" s="2">
+        <v>61.11</v>
+      </c>
+      <c r="M40" s="2">
+        <v>38.630000000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>21</v>
       </c>
@@ -2108,7 +5701,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>61</v>
       </c>
@@ -2137,7 +5730,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>62</v>
       </c>
@@ -2166,7 +5759,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>63</v>
       </c>
@@ -2195,7 +5788,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>64</v>
       </c>
@@ -2224,7 +5817,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>65</v>
       </c>
@@ -2253,7 +5846,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>66</v>
       </c>
@@ -2282,12 +5875,12 @@
         <v>129</v>
       </c>
     </row>
-    <row r="48" spans="1:9" s="9" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" s="9" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>36</v>
       </c>
@@ -2315,8 +5908,20 @@
       <c r="I49" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J49" s="2">
+        <v>18.12</v>
+      </c>
+      <c r="K49" s="2">
+        <v>20.3</v>
+      </c>
+      <c r="L49" s="2">
+        <v>61.11</v>
+      </c>
+      <c r="M49" s="2">
+        <v>38.630000000000003</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>37</v>
       </c>
@@ -2344,8 +5949,20 @@
       <c r="I50" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J50" s="2">
+        <v>39.450000000000003</v>
+      </c>
+      <c r="K50" s="2">
+        <v>39.75</v>
+      </c>
+      <c r="L50" s="2">
+        <v>61.11</v>
+      </c>
+      <c r="M50" s="2">
+        <v>38.630000000000003</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>38</v>
       </c>
@@ -2373,8 +5990,20 @@
       <c r="I51" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J51" s="2">
+        <v>78.8</v>
+      </c>
+      <c r="K51" s="2">
+        <v>79.14</v>
+      </c>
+      <c r="L51" s="2">
+        <v>61.11</v>
+      </c>
+      <c r="M51" s="2">
+        <v>38.630000000000003</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>39</v>
       </c>
@@ -2402,8 +6031,20 @@
       <c r="I52" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J52" s="2">
+        <v>95.24</v>
+      </c>
+      <c r="K52" s="2">
+        <v>95.46</v>
+      </c>
+      <c r="L52" s="2">
+        <v>61.11</v>
+      </c>
+      <c r="M52" s="2">
+        <v>38.630000000000003</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>40</v>
       </c>
@@ -2431,8 +6072,20 @@
       <c r="I53" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J53" s="2">
+        <v>98.69</v>
+      </c>
+      <c r="K53" s="2">
+        <v>99.09</v>
+      </c>
+      <c r="L53" s="2">
+        <v>61.11</v>
+      </c>
+      <c r="M53" s="2">
+        <v>38.630000000000003</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>41</v>
       </c>
@@ -2461,7 +6114,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>42</v>
       </c>
@@ -2490,7 +6143,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>43</v>
       </c>
@@ -2519,7 +6172,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>44</v>
       </c>
@@ -2548,7 +6201,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>45</v>
       </c>
@@ -2577,7 +6230,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>46</v>
       </c>
@@ -2606,7 +6259,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>47</v>
       </c>
@@ -2635,7 +6288,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>48</v>
       </c>
@@ -2664,7 +6317,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>49</v>
       </c>
@@ -2693,7 +6346,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>50</v>
       </c>
@@ -2722,7 +6375,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>51</v>
       </c>
@@ -3013,7 +6666,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="L1:M1"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="I1:I2"/>
@@ -3027,5 +6681,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add report and presentation file
</commit_message>
<xml_diff>
--- a/MySEProject/Dataset Reports/Dataset-GurunagSai/Experiment Report.xlsx
+++ b/MySEProject/Dataset Reports/Dataset-GurunagSai/Experiment Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gurunag Sai\source\repos\neocortexapi-classification\MySEProject\Dataset Reports\Dataset-GurunagSai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22130B3A-4858-471D-9529-68FBDE653F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D081C40-1C35-46CF-AA4C-DD08FA9B18D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="148">
   <si>
     <t>Experiment Number</t>
   </si>
@@ -147,10 +147,6 @@
 macro corelation(36-1.8%) micro corelation(81-40%)</t>
   </si>
   <si>
-    <t>Valid output
-macro corelation(57-17%) micro corelation(89-64%)</t>
-  </si>
-  <si>
     <t>output-21</t>
   </si>
   <si>
@@ -485,15 +481,76 @@
     <t>valid output macro corelation(46-4%) micro corelation(87-47%)</t>
   </si>
   <si>
-    <t>Better output micro(92-75) and macro(68-45)</t>
+    <t>Experiments  with potential radiius 1</t>
+  </si>
+  <si>
+    <t>output-67</t>
+  </si>
+  <si>
+    <t>output-68</t>
+  </si>
+  <si>
+    <t>output-69</t>
+  </si>
+  <si>
+    <t>output-70</t>
+  </si>
+  <si>
+    <t>output-71</t>
+  </si>
+  <si>
+    <t>output-72</t>
+  </si>
+  <si>
+    <t>output-73</t>
+  </si>
+  <si>
+    <t>output-74</t>
+  </si>
+  <si>
+    <t>variance is very high between the max and min value</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">BEST OUTPUT </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>macro corelation(57-17%) micro corelation(89-64%)</t>
+    </r>
+  </si>
+  <si>
+    <t>valid output micro(92-75) and macro(68-45)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -598,7 +655,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -618,15 +675,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -645,6 +693,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -925,10 +983,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:I82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O84" sqref="O84"/>
+    <sheetView tabSelected="1" topLeftCell="D49" workbookViewId="0">
+      <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,24 +1004,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>61</v>
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="4" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
+      <c r="A2" s="11"/>
       <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
@@ -977,17 +1035,17 @@
         <v>2</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="16"/>
-    </row>
-    <row r="3" spans="1:9" s="9" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>130</v>
+        <v>98</v>
+      </c>
+      <c r="H2" s="14"/>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="3" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1158,7 +1216,7 @@
         <v>5</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>19</v>
@@ -1187,7 +1245,7 @@
         <v>5</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>19</v>
@@ -1216,7 +1274,7 @@
         <v>5</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>19</v>
@@ -1239,16 +1297,16 @@
         <v>10</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1268,16 +1326,16 @@
         <v>20</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1297,16 +1355,16 @@
         <v>50</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1326,16 +1384,16 @@
         <v>100</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1355,16 +1413,16 @@
         <v>10</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1384,16 +1442,16 @@
         <v>50</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1413,16 +1471,16 @@
         <v>100</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1448,10 +1506,10 @@
         <v>5</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1477,10 +1535,10 @@
         <v>5</v>
       </c>
       <c r="H20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I20" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1506,15 +1564,15 @@
         <v>5</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" s="9" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>131</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1630,7 +1688,7 @@
         <v>22</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1659,7 +1717,7 @@
         <v>23</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1679,30 +1737,30 @@
         <v>100</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" s="9" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
     </row>
     <row r="30" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
@@ -1730,7 +1788,7 @@
         <v>13</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1759,7 +1817,7 @@
         <v>24</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1849,9 +1907,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="9" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
-        <v>134</v>
+    <row r="35" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1880,7 +1938,7 @@
         <v>14</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1908,8 +1966,8 @@
       <c r="H37" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I37" s="2" t="s">
-        <v>37</v>
+      <c r="I37" s="1" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2022,10 +2080,10 @@
         <v>5</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>52</v>
+        <v>37</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2051,10 +2109,10 @@
         <v>5</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2080,10 +2138,10 @@
         <v>5</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2109,10 +2167,10 @@
         <v>5</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2138,10 +2196,10 @@
         <v>5</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2167,10 +2225,10 @@
         <v>5</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2196,15 +2254,15 @@
         <v>5</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" s="9" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
-        <v>133</v>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="15" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2230,10 +2288,10 @@
         <v>5</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2259,10 +2317,10 @@
         <v>5</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2288,10 +2346,10 @@
         <v>5</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2317,10 +2375,10 @@
         <v>5</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2346,10 +2404,10 @@
         <v>5</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2375,10 +2433,10 @@
         <v>5</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2404,10 +2462,10 @@
         <v>5</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2433,10 +2491,10 @@
         <v>5</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2462,10 +2520,10 @@
         <v>5</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2491,10 +2549,10 @@
         <v>5</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2520,10 +2578,10 @@
         <v>5</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2549,10 +2607,10 @@
         <v>5</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2578,10 +2636,10 @@
         <v>5</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2607,10 +2665,10 @@
         <v>5</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2636,10 +2694,10 @@
         <v>5</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2665,10 +2723,10 @@
         <v>5</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2694,10 +2752,10 @@
         <v>5</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2723,10 +2781,10 @@
         <v>5</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2752,10 +2810,10 @@
         <v>5</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2781,10 +2839,10 @@
         <v>5</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2810,10 +2868,10 @@
         <v>5</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2839,10 +2897,10 @@
         <v>5</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2868,10 +2926,10 @@
         <v>5</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2897,10 +2955,10 @@
         <v>5</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2926,23 +2984,261 @@
         <v>5</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="15" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="18">
+        <v>67</v>
+      </c>
+      <c r="B75" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C75" s="18">
+        <v>1</v>
+      </c>
+      <c r="D75" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="E75" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H75" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="18">
+        <v>68</v>
+      </c>
+      <c r="B76" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C76" s="18">
+        <v>1</v>
+      </c>
+      <c r="D76" s="18">
+        <v>0.2</v>
+      </c>
+      <c r="E76" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H76" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="18">
+        <v>69</v>
+      </c>
+      <c r="B77" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C77" s="18">
+        <v>1</v>
+      </c>
+      <c r="D77" s="18">
+        <v>0.3</v>
+      </c>
+      <c r="E77" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H77" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="18">
+        <v>70</v>
+      </c>
+      <c r="B78" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C78" s="18">
+        <v>1</v>
+      </c>
+      <c r="D78" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="E78" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H78" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="18">
+        <v>71</v>
+      </c>
+      <c r="B79" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C79" s="18">
+        <v>1</v>
+      </c>
+      <c r="D79" s="18">
+        <v>0.6</v>
+      </c>
+      <c r="E79" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H79" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="18">
+        <v>72</v>
+      </c>
+      <c r="B80" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C80" s="18">
+        <v>1</v>
+      </c>
+      <c r="D80" s="18">
+        <v>0.7</v>
+      </c>
+      <c r="E80" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H80" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="I80" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="18">
+        <v>73</v>
+      </c>
+      <c r="B81" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C81" s="18">
+        <v>1</v>
+      </c>
+      <c r="D81" s="18">
+        <v>0.8</v>
+      </c>
+      <c r="E81" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H81" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="18">
+        <v>74</v>
+      </c>
+      <c r="B82" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C82" s="18">
+        <v>1</v>
+      </c>
+      <c r="D82" s="18">
+        <v>0.9</v>
+      </c>
+      <c r="E82" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H82" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="A22:XFD22"/>
+    <mergeCell ref="A29:XFD29"/>
+    <mergeCell ref="A35:XFD35"/>
+    <mergeCell ref="A48:XFD48"/>
+    <mergeCell ref="A74:XFD74"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="A3:XFD3"/>
-    <mergeCell ref="A22:XFD22"/>
-    <mergeCell ref="A29:XFD29"/>
-    <mergeCell ref="A35:XFD35"/>
-    <mergeCell ref="A48:XFD48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>